<commit_message>
Fixed a couple of bugs from the GET fix.  Prepared POST route to insert massImport entries
</commit_message>
<xml_diff>
--- a/mass_input_template.xlsx
+++ b/mass_input_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JLow/Desktop/ticklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B761743-432F-6A45-AE80-AAAE254E4F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80D9BD0-159C-004A-A934-10ED709DCA84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15960" xr2:uid="{B8D7F496-9133-5241-B223-25D63E55584D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Area1</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>trad</t>
+  </si>
+  <si>
+    <t>Aid_Grade</t>
   </si>
 </sst>
 </file>
@@ -489,15 +492,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2B3B19-0536-B040-BB15-BD3DB4E34A4B}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,34 +529,37 @@
         <v>16</v>
       </c>
       <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -581,23 +587,23 @@
       <c r="I2">
         <v>4</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>4</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -619,25 +625,25 @@
       <c r="I3" t="s">
         <v>33</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>8</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>34</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>650</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>4</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>